<commit_message>
modified:   Brighway/Results/Ananas sub - CONSQ.xlsx 	modified:   Brighway/Rune BE.ipynb
</commit_message>
<xml_diff>
--- a/Brighway/Results/Ananas sub - CONSQ.xlsx
+++ b/Brighway/Results/Ananas sub - CONSQ.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="163">
   <si>
     <t>('EF v3.1 EN15804', 'acidification', 'accumulated exceedance (AE)')</t>
   </si>
@@ -64,148 +64,445 @@
     <t>('EF v3.1 EN15804', 'water use', 'user deprivation potential (deprivation-weighted water consumption)')</t>
   </si>
   <si>
-    <t>[["Steel cylinder", 2.8068814282309142e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0015934554489910667]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.033706295500991905], ["Steel cylinder", 2.8068814282309142e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase CDU", 0.0011995761189752317], ["EoL CDU", 0.009568273319826437], ["EoL 50L cylinder - FU", 0.0015934554489910667]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.0690910181269958], ["Steel cylinder", 2.8068814282309142e-05], ["nitrous oxide production", 0.010968005818038482], ["Use phase MDU", 0.0004519679633273833], ["EoL MDU", 0.023743427245292378], ["EoL 50L cylinder - FU", 0.0015934554489910667]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.006277467071218475], ["nitrous oxide production", 2.7735767368862367], ["Use phase basecase", 227.34409189224243], ["EoL 50L cylinder - FU", 1.3797549867462602]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.12905040685291852], ["Steel cylinder", 0.006277467071218475], ["nitrous oxide production", 2.7735767368862367], ["Use phase CDU", 43.44535637749612], ["EoL CDU", -0.010913517128917348], ["EoL 50L cylinder - FU", 1.3797549867462602]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.3591249305157672], ["Steel cylinder", 0.006277467071218475], ["nitrous oxide production", 2.7735767368862367], ["Use phase MDU", 43.404329830374245], ["EoL MDU", -0.028320516611116342], ["EoL 50L cylinder - FU", 1.3797549867462602]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.03152632186590881], ["nitrous oxide production", 15.635308294302359], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 2.596880647098815]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 1.4899964112890802], ["Steel cylinder", 0.03152632186590881], ["nitrous oxide production", 15.635308294302359], ["Use phase CDU", 0.7412027382979668], ["EoL CDU", -0.21693100903846793], ["EoL 50L cylinder - FU", 2.596880647098815]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 5.562379936011466], ["Steel cylinder", 0.03152632186590881], ["nitrous oxide production", 15.635308294302359], ["Use phase MDU", 0.2792652227250268], ["EoL MDU", -0.5284116708803903], ["EoL 50L cylinder - FU", 2.596880647098815]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.07842803132504617], ["nitrous oxide production", 46.31028189903245], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 6.953517004960654]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 2.1050843577039284], ["Steel cylinder", 0.07842803132504617], ["nitrous oxide production", 46.31028189903245], ["Use phase CDU", 0.6692525251663012], ["EoL CDU", -0.09497370330413925], ["EoL 50L cylinder - FU", 6.953517004960654]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 5.548337101555568], ["Steel cylinder", 0.07842803132504617], ["nitrous oxide production", 46.31028189903245], ["Use phase MDU", 0.2521563208589757], ["EoL MDU", -0.22894948284262986], ["EoL 50L cylinder - FU", 6.953517004960654]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 4.435636453485354e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.00012311536066591725]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.00011021647529885492], ["Steel cylinder", 4.435636453485354e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase CDU", 2.849641883711377e-05], ["EoL CDU", -2.051417753377876e-05], ["EoL 50L cylinder - FU", 0.00012311536066591725]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.0003663742164220076], ["Steel cylinder", 4.435636453485354e-06], ["nitrous oxide production", 0.0009169092173445685], ["Use phase MDU", 1.0736682883398692e-05], ["EoL MDU", -4.919735864856039e-05], ["EoL 50L cylinder - FU", 0.00012311536066591725]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 6.988203678348106e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.000653739484881074]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.0001277696567481476], ["Steel cylinder", 6.988203678348106e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase CDU", 0.0002792513031362428], ["EoL CDU", -7.792099234694213e-05], ["EoL 50L cylinder - FU", 0.000653739484881074]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.0003618564128267861], ["Steel cylinder", 6.988203678348106e-06], ["nitrous oxide production", 0.005230909219588117], ["Use phase MDU", 0.00010521436759080808], ["EoL MDU", -0.0001918865112239045], ["EoL 50L cylinder - FU", 0.000653739484881074]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 6.029305097784666e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.004205256080212307]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.001305192214177572], ["Steel cylinder", 6.029305097784666e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase CDU", 0.00435189277730263], ["EoL CDU", -0.0011410749274370425], ["EoL 50L cylinder - FU", 0.004205256080212307]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.00376108667227394], ["Steel cylinder", 6.029305097784666e-05], ["nitrous oxide production", 0.029899230463375122], ["Use phase MDU", 0.0016396759522497191], ["EoL MDU", -0.0028112447635443957], ["EoL 50L cylinder - FU", 0.004205256080212307]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 8.161609885996017e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 2.454274505775019e-10]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 3.243928866899465e-10], ["Steel cylinder", 8.161609885996017e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase CDU", 3.112433080829649e-10], ["EoL CDU", -1.382464959096833e-10], ["EoL 50L cylinder - FU", 2.454274505775019e-10]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 1.0716849153781413e-09], ["Steel cylinder", 8.161609885996017e-11], ["nitrous oxide production", 1.3815806307562065e-09], ["Use phase MDU", 1.1726809314424572e-10], ["EoL MDU", -3.4273432030762576e-10], ["EoL 50L cylinder - FU", 2.454274505775019e-10]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 7.530671062658518e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase basecase", 1.3361670158765134e-08], ["EoL 50L cylinder - FU", 5.055227005763586e-09]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 4.681941563932091e-09], ["Steel cylinder", 7.530671062658518e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase CDU", 1.1108940558494202e-08], ["EoL CDU", -7.86491525690251e-09], ["EoL 50L cylinder - FU", 5.055227005763586e-09]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 1.1984131040941075e-08], ["Steel cylinder", 7.530671062658518e-11], ["nitrous oxide production", 2.7210021087733674e-08], ["Use phase MDU", 5.774491740088175e-09], ["EoL MDU", -1.9440126151375635e-08], ["EoL 50L cylinder - FU", 5.055227005763586e-09]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.00016032698705349696], ["nitrous oxide production", 0.42490983327819815], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.05221819451590624]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.02299027511022214], ["Steel cylinder", 0.00016032698705349696], ["nitrous oxide production", 0.42490983327819815], ["Use phase CDU", 0.0003478036811559822], ["EoL CDU", 0.0005368187911133735], ["EoL 50L cylinder - FU", 0.05221819451590624]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.05186765582859973], ["Steel cylinder", 0.00016032698705349696], ["nitrous oxide production", 0.42490983327819815], ["Use phase MDU", 0.00013104305672618255], ["EoL MDU", 0.0013724670382122136], ["EoL 50L cylinder - FU", 0.05221819451590624]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.061935905197313214], ["nitrous oxide production", 28.792690550160245], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 4.553405137576023]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 1.4517019264400177], ["Steel cylinder", 0.061935905197313214], ["nitrous oxide production", 28.792690550160245], ["Use phase CDU", 30.062931902825287], ["EoL CDU", -0.5926562572475528], ["EoL 50L cylinder - FU", 4.553405137576023]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 3.6900959245079963], ["Steel cylinder", 0.061935905197313214], ["nitrous oxide production", 28.792690550160245], ["Use phase MDU", 11.326902802466671], ["EoL MDU", -1.4269104476387922], ["EoL 50L cylinder - FU", 4.553405137576023]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", -5.216055093358714e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 5.124795543368275e-06]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 2.336491107311484e-05], ["Steel cylinder", -5.216055093358714e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase CDU", 9.734411970101328e-06], ["EoL CDU", -6.048185424361905e-06], ["EoL 50L cylinder - FU", 5.124795543368275e-06]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 7.762141349179897e-05], ["Steel cylinder", -5.216055093358714e-08], ["nitrous oxide production", 3.528425210128439e-05], ["Use phase MDU", 3.6676641713034824e-06], ["EoL MDU", -1.4385742203969544e-05], ["EoL 50L cylinder - FU", 5.124795543368275e-06]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 1.4852521528980564e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 1.0432841391810307e-07]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 6.448093853719628e-09], ["Steel cylinder", 1.4852521528980564e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase CDU", 1.9450074606027338e-09], ["EoL CDU", 7.567022242406086e-12], ["EoL 50L cylinder - FU", 1.0432841391810307e-07]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 1.8962760185799554e-08], ["Steel cylinder", 1.4852521528980564e-10], ["nitrous oxide production", 8.530261057304866e-08], ["Use phase MDU", 7.328264098676998e-10], ["EoL MDU", 1.5588458631096705e-11], ["EoL 50L cylinder - FU", 1.0432841391810307e-07]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 5.651607932546053e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 1.6048194601713715e-08]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 2.9230755321320073e-08], ["Steel cylinder", 5.651607932546053e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase CDU", 1.3992546509704515e-08], ["EoL CDU", 5.258378664716782e-09], ["EoL 50L cylinder - FU", 1.6048194601713715e-08]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 6.342169280575578e-08], ["Steel cylinder", 5.651607932546053e-10], ["nitrous oxide production", 5.905655038504484e-08], ["Use phase MDU", 5.272014545569526e-09], ["EoL MDU", 1.3037019606857843e-08], ["EoL 50L cylinder - FU", 1.6048194601713715e-08]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 2.543154265658326e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.0012673930564333607]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.0026820678763302087], ["Steel cylinder", 2.543154265658326e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase CDU", 0.0008604984653688513], ["EoL CDU", 0.00034483736920948576], ["EoL 50L cylinder - FU", 0.0012673930564333607]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.005810953630409368], ["Steel cylinder", 2.543154265658326e-05], ["nitrous oxide production", 0.007059262000778557], ["Use phase MDU", 0.00032421263868720836], ["EoL MDU", 0.0008591276393808767], ["EoL 50L cylinder - FU", 0.0012673930564333607]]</t>
-  </si>
-  <si>
-    <t>[["Steel cylinder", 0.002827557969478974], ["nitrous oxide production", 4.430496838846222], ["Use phase basecase", 0.0], ["EoL 50L cylinder - FU", 0.4699444627032996]]</t>
-  </si>
-  <si>
-    <t>[["CDU updated", 0.04630923474954789], ["Steel cylinder", 0.002827557969478974], ["nitrous oxide production", 4.430496838846222], ["Use phase CDU", 0.026577952308437253], ["EoL CDU", 0.005541157071511327], ["EoL 50L cylinder - FU", 0.4699444627032996]]</t>
-  </si>
-  <si>
-    <t>[["MDU updated", 0.12369240377069371], ["Steel cylinder", 0.002827557969478974], ["nitrous oxide production", 4.430496838846222], ["Use phase MDU", 0.01001385638163526], ["EoL MDU", 0.01385106430137736], ["EoL 50L cylinder - FU", 0.4699444627032996]]</t>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 1.1176280771220774e-07], ["'Steel cylinder prod.' (unit, GLO, None)", 2.277291346205234e-05], ["'Hydrastic testing 50L' (unit, GLO, None)", 1.5561269172951786e-06], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 3.434578940649671e-07], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 3.699990455344564e-08], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 0.0095143137313242]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase basecase' (unit, GLO, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 0.0001309840220531174], ["'nitrous oxide production' (kilogram, RER, None)", 0.0010976730169166898], ["'Cylinder maintenance 50L' (unit, GLO, None)", 7.36071265804377e-05], ["'Hydrastic testing 50L' (unit, GLO, None)", 1.4005142257549842e-05], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -2.5750144930587655e-07], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.00021635988593489902], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 2.3307937500084964e-05], ["'Compresser opration 50L' (unit, GLO, None)", 3.777582899872765e-05]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.00024151655784523075], ["'injection moulding' (kilogram, RER, None)", 2.2546388830490307e-07], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 8.380391549553054e-05], ["'market for sodium silicate, solid' (kilogram, RER, None)", 1.237959490025488e-06], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 1.0973006377467984e-05], ["'polypropylene production, granulate' (kilogram, RER, None)", 4.2938369614454936e-07], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 6.247413638142965e-05], ["'Coating' (kilogram, GLO, None)", 0.0332991030605314]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 0.0011995761189071566], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.0011995761473321714]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 0.0002509936985151429], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 7.688172986127888e-07], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -1.0705332815300094e-06], ["'waste electronics' (kilogram, GLO, None)", 0.0009520099514795484], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", 1.823381088013175e-05], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 3.33650580272967e-06]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.0005138650166921101], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 1.8825026162789532e-05], ["'injection moulding' (kilogram, RER, None)", 6.87128040544631e-07], ["'market for acetaldehyde' (kilogram, GLO, None)", 1.323423514833032e-07], ["'market for nylon 6' (kilogram, RER, None)", 9.913979260722098e-07], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.0016760783099087505], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 6.407600123877821e-06], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 4.0216068373875656e-05], ["'polypropylene production, granulate' (kilogram, RER, None)", 1.0631975427108182e-06], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.00022896770984274362], ["'synthetic rubber production' (kilogram, RER, None)", 5.580603076830654e-06], ["'Coating' (kilogram, GLO, None)", 0.06659820612105596]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 0.00045196796330177], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.00045196796331220925]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 0.0050198739703033795], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 2.34306224339146e-06], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -3.92350447680883e-06], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 4.904309971181766e-06], ["'waste electronics' (kilogram, GLO, None)", 0.002025553088254359], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 6.673011605472232e-06]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 1.6506026376331343e-05], ["'Steel cylinder prod.' (unit, GLO, None)", 0.004965675918395517], ["'Hydrastic testing 50L' (unit, GLO, None)", 0.0002986988027667966], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.00017103437440246975], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 4.314397150294659e-06], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 2.405968748621886]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase basecase' (unit, GLO, None)", 227.34409189224243]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 0.02667376660028759], ["'nitrous oxide production' (kilogram, RER, None)", 0.27757829408186957], ["'Cylinder maintenance 50L' (unit, GLO, None)", 0.008783854484338664], ["'Hydrastic testing 50L' (unit, GLO, None)", 0.0026882892249607037], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -2.9034012275637426e-05], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.1077423997994092], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 0.0027178367172370414], ["'Compresser opration 50L' (unit, GLO, None)", 0.0055790369151272135]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.03740152231968872], ["'injection moulding' (kilogram, RER, None)", 8.980857850917068e-05], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.003601423082995224], ["'market for sodium silicate, solid' (kilogram, RER, None)", 0.00018110038081648857], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.0036145243224257936], ["'polypropylene production, granulate' (kilogram, RER, None)", 0.00013313607456191562], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.013123701355041872], ["'Coating' (kilogram, GLO, None)", 0.07005305069653145]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 43.445356377489226], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.06582922746516492]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -0.00027980006204120277], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", -7.463380727876748e-05], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -0.00012070563688568935], ["'waste electronics' (kilogram, GLO, None)", -0.00031953250701686694], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", -1.4033435324626067e-05], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.0005061235537199164]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.07957770706322907], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 0.002973651635966743], ["'injection moulding' (kilogram, RER, None)", 0.0002737023345039819], ["'market for acetaldehyde' (kilogram, GLO, None)", 3.186253150230851e-05], ["'market for nylon 6' (kilogram, RER, None)", 0.0002559417571387803], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.07202846165927654], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 0.0008212427387063568], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.013247231641949013], ["'polypropylene production, granulate' (kilogram, RER, None)", 0.0003296584117913119], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.04809836546625092], ["'synthetic rubber production' (kilogram, RER, None)", 0.0013810055320252349], ["'Coating' (kilogram, GLO, None)", 0.14010610139263904]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 43.404329830371644], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.024802678787850797]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -0.005596001240705667], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", -0.00022745541265909992], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -0.0004423861591864381], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", -0.0011651925766969164], ["'waste electronics' (kilogram, GLO, None)", -0.0006798563979086753], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.0010122471074393]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 5.709188492838599e-05], ["'Steel cylinder prod.' (unit, GLO, None)", 0.022773511714858953], ["'Hydrastic testing 50L' (unit, GLO, None)", 0.0028947611619163], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.0011495134804026183], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 2.1933242220265765e-05], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 13.56301508844953]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 0.1371946158645319], ["'nitrous oxide production' (kilogram, RER, None)", 1.5647745187905489], ["'Cylinder maintenance 50L' (unit, GLO, None)", 0.11179387356114838], ["'Hydrastic testing 50L' (unit, GLO, None)", 0.026052850457911742], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -0.0001802735962888466], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.7241312830422768], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 0.0138167556109802], ["'Compresser opration 50L' (unit, GLO, None)", 0.019297057099687983]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 1.0777622051641287], ["'injection moulding' (kilogram, RER, None)", 0.00011156607493174284], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.129626556845388], ["'market for sodium silicate, solid' (kilogram, RER, None)", 0.003950984001074506], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.019328494491990835], ["'polypropylene production, granulate' (kilogram, RER, None)", 0.00011232139771114223], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.04396235222892055], ["'Coating' (kilogram, GLO, None)", 0.20067912574767574]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 0.7412027382264046], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.7412027557978251]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -0.005146077004981382], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", -0.0001710462398349003], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -0.0007494671782570551], ["'waste electronics' (kilogram, GLO, None)", 0.001114591329724848], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", -0.0004830019417873384], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.0008081235400536305]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 2.293111074817628], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 0.005466387601977658], ["'injection moulding' (kilogram, RER, None)", 0.00034001089503017386], ["'market for acetaldehyde' (kilogram, GLO, None)", 4.331692352843698e-05], ["'market for nylon 6' (kilogram, RER, None)", 0.00012606603305840338], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 2.5925311369056345], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 0.02113864202464903], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.07083893231401903], ["'polypropylene production, granulate' (kilogram, RER, None)", 0.0002781191626839545], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.16112202091955558], ["'synthetic rubber production' (kilogram, RER, None)", 0.01602592285308242], ["'Coating' (kilogram, GLO, None)", 0.40135825149066334]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 0.2792652226980472], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.27926522270753007]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -0.10292154009912408], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", -0.0005212837785445274], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -0.002746797208313956], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", -0.0016014763024597388], ["'waste electronics' (kilogram, GLO, None)", 0.002371470914309809], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.0016162470801040938]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 0.00030992122254397354], ["'Steel cylinder prod.' (unit, GLO, None)", 0.05627107770498489], ["'Hydrastic testing 50L' (unit, GLO, None)", 0.005659473394083347], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.002423623626017584], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 5.1770118247744625e-05], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 40.17234840055018]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 0.5061069437938703], ["'nitrous oxide production' (kilogram, RER, None)", 4.634711878353885], ["'Cylinder maintenance 50L' (unit, GLO, None)", 0.0980293113566386], ["'Hydrastic testing 50L' (unit, GLO, None)", 0.05093526054763944], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -0.0003837862970203554], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 1.5267517222193814], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 0.03261237278998965], ["'Compresser opration 50L' (unit, GLO, None)", 0.10475337321958011]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.5055865764257307], ["'injection moulding' (kilogram, RER, None)", 0.0016415858658482372], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.0491639470602572], ["'market for sodium silicate, solid' (kilogram, RER, None)", 0.0016566688726974488], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.0440123743222368], ["'polypropylene production, granulate' (kilogram, RER, None)", 0.005166672849550641], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.14581438001534752], ["'Coating' (kilogram, GLO, None)", 1.3412468856918016]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 0.6692525250789959], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.6692525409504394]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -0.0024287058125342987], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 0.001000827837015995], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -0.0015955483165755527], ["'waste electronics' (kilogram, GLO, None)", 0.0005278808315993609], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", 4.493533980585124e-05], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.004812967094318461]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 1.0757161200550822], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 0.04103871429033195], ["'injection moulding' (kilogram, RER, None)", 0.005002928353059287], ["'market for acetaldehyde' (kilogram, GLO, None)", 0.0008156529948038325], ["'market for nylon 6' (kilogram, RER, None)", 0.003172806929831131], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.9832789411972744], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 0.0061107346312871446], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.16130535189429906], ["'polypropylene production, granulate' (kilogram, RER, None)", 0.012793205533727169], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.5344097027564197], ["'synthetic rubber production' (kilogram, RER, None)", 0.042199226079627505], ["'Coating' (kilogram, GLO, None)", 2.6824937713782955]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 0.2521563208261186], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.25215632083682843]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -0.04857411624921576], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 0.003050141979477321], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -0.00584768458025326], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.0063452252850996], ["'waste electronics' (kilogram, GLO, None)", 0.0011231507055316486], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.009625934188631275]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 1.1376311728602588e-08], ["'Steel cylinder prod.' (unit, GLO, None)", 3.898474300101073e-06], ["'Hydrastic testing 50L' (unit, GLO, None)", 2.3623789425234415e-07], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 1.7499800070920315e-08], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 5.574494456417174e-10], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 0.0007953826886718914]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 1.4739829756467497e-05], ["'nitrous oxide production' (kilogram, RER, None)", 9.176385603188705e-05], ["'Cylinder maintenance 50L' (unit, GLO, None)", -7.337609458213927e-07], ["'Hydrastic testing 50L' (unit, GLO, None)", 2.1261410483064892e-06], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -9.880398392651137e-10], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 1.1023926986787447e-05], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 3.511629825890657e-07], ["'Compresser opration 50L' (unit, GLO, None)", 3.84519336441869e-06]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 5.9158109354219824e-05], ["'injection moulding' (kilogram, RER, None)", 2.4979322505563832e-08], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 6.509117845636389e-06], ["'market for sodium silicate, solid' (kilogram, RER, None)", 1.960510995646629e-07], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 1.6303100914088047e-06], ["'polypropylene production, granulate' (kilogram, RER, None)", 1.0766245680634232e-08], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 1.0561468208790006e-05], ["'Coating' (kilogram, GLO, None)", 3.1374985673283934e-05]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 2.849641883337073e-05], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 2.8496419509058757e-05]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -5.137465795963295e-07], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 1.5452893434527127e-07], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -4.107664381271501e-09], ["'waste electronics' (kilogram, GLO, None)", -4.5209360618646596e-07], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", -1.846171077192829e-08], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 1.734926090236577e-07]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.0001258683177749535], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 1.3883372080497149e-06], ["'injection moulding' (kilogram, RER, None)", 7.61274590645154e-08], ["'market for acetaldehyde' (kilogram, GLO, None)", 1.3475729890524258e-08], ["'market for nylon 6' (kilogram, RER, None)", 4.445357170290244e-09], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.00013018235691235604], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 1.0006253602595005e-06], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 5.975086485155692e-06], ["'polypropylene production, granulate' (kilogram, RER, None)", 2.6658315289590047e-08], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 3.870778098534502e-05], ["'synthetic rubber production' (kilogram, RER, None)", 3.810313847073756e-07], ["'Coating' (kilogram, GLO, None)", 6.274997134631633e-05]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 1.073668288198834e-05], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 1.0736682882404605e-05]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -1.027493159193603e-05], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 4.709453237189215e-07], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -1.505458995752763e-08], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 9.441800223557808e-07], ["'waste electronics' (kilogram, GLO, None)", -9.619012897583598e-07], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 3.4698521804697055e-07]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 1.690958326088436e-08], ["'Steel cylinder prod.' (unit, GLO, None)", 4.575322107204184e-06], ["'Hydrastic testing 50L' (unit, GLO, None)", 7.359982710538787e-07], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 9.407725304337311e-08], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 1.7059165638444613e-08], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 0.004537608043068941]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 3.468551015271597e-05], ["'nitrous oxide production' (kilogram, RER, None)", 0.0005235070075256874], ["'Cylinder maintenance 50L' (unit, GLO, None)", 1.3320563309728485e-05], ["'Hydrastic testing 50L' (unit, GLO, None)", 6.623984439620341e-06], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -1.2294631609730916e-07], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 5.926357812481954e-05], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 1.0746351140720611e-05], ["'Compresser opration 50L' (unit, GLO, None)", 5.715439141658421e-06]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 4.857972049159303e-05], ["'injection moulding' (kilogram, RER, None)", 4.219045961512965e-08], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 4.407468041251715e-06], ["'market for sodium silicate, solid' (kilogram, RER, None)", 1.7491464755650228e-07], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 3.0536491543453037e-06], ["'polypropylene production, granulate' (kilogram, RER, None)", 8.206147118667505e-08], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 1.1947841773817733e-05], ["'Coating' (kilogram, GLO, None)", 5.495160359567171e-05]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 0.00027925130312526306], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.0002792513097399328]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -1.9849153700335424e-06], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 1.0893169196792552e-07], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -5.111354657551273e-07], ["'waste electronics' (kilogram, GLO, None)", -4.286927451417271e-06], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", -1.1818267353658035e-07], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 5.481182061142123e-07]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.00010336110742896427], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 2.758992636453233e-06], ["'injection moulding' (kilogram, RER, None)", 1.285804483509161e-07], ["'market for acetaldehyde' (kilogram, GLO, None)", 2.822830699278722e-08], ["'market for nylon 6' (kilogram, RER, None)", 2.7476522499468043e-07], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 8.814936082456689e-05], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 9.643958578412443e-07], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 1.119162415086071e-05], ["'polypropylene production, granulate' (kilogram, RER, None)", 2.0319251825400468e-07], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 4.378884010122396e-05], ["'synthetic rubber production' (kilogram, RER, None)", 1.1041184589940173e-06], ["'Coating' (kilogram, GLO, None)", 0.00010990320719058]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 0.00010521436758666906], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.00010521436758818682]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -3.969830740062019e-05], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 3.31982299330814e-07], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -1.8733114819928985e-06], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 7.317836862328858e-07], ["'waste electronics' (kilogram, GLO, None)", -9.121122237057771e-06], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 1.0962364122277184e-06]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 1.80731103446373e-07], ["'Steel cylinder prod.' (unit, GLO, None)", 4.721946976783688e-05], ["'Hydrastic testing 50L' (unit, GLO, None)", 2.898202202100958e-06], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 9.562687729369905e-07], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 1.854166095754906e-07], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 0.025936406642743555]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 0.00028305148820988895], ["'nitrous oxide production' (kilogram, RER, None)", 0.002992301339996172], ["'Cylinder maintenance 50L' (unit, GLO, None)", 0.00012486950982516372], ["'Hydrastic testing 50L' (unit, GLO, None)", 2.6083819820856225e-05], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -1.3371688393145078e-06], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.00060239757539662], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 0.00011680242961765472], ["'Compresser opration 50L' (unit, GLO, None)", 6.108711295033925e-05]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.0005127941885006088], ["'injection moulding' (kilogram, RER, None)", 3.8527257276048695e-07], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 4.464280294383637e-05], ["'market for sodium silicate, solid' (kilogram, RER, None)", 2.8645444503208226e-06], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 2.6284837800522982e-05], ["'polypropylene production, granulate' (kilogram, RER, None)", 8.84567405157784e-07], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.00012758782039416343], ["'Coating' (kilogram, GLO, None)", 0.0005763612423640631]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 0.004351892777136212], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.004351892880220733]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -2.9085166453694612e-05], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 1.0541330769128852e-06], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -5.559128887890294e-06], ["'waste electronics' (kilogram, GLO, None)", -6.342497960142116e-05], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", -1.8297968751111913e-06], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 5.770261655924443e-06]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.0010910514648956944], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 2.7637513792407562e-05], ["'injection moulding' (kilogram, RER, None)", 1.174164031270919e-06], ["'market for acetaldehyde' (kilogram, GLO, None)", 2.873234736277786e-07], ["'market for nylon 6' (kilogram, RER, None)", 2.256867569972126e-06], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.0008928560588718011], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 1.5827775328610714e-05], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 9.633393054089065e-05], ["'polypropylene production, granulate' (kilogram, RER, None)", 2.1902785316948594e-06], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.0004676093617480315], ["'synthetic rubber production' (kilogram, RER, None)", 1.1139453435860389e-05], ["'Coating' (kilogram, GLO, None)", 0.0011527224847164787]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 0.0016396759521870126], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.0016396759522108667]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -0.0005817033290733367], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 3.212596043924987e-06], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -2.0374207374121993e-05], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 7.027064242675754e-06], ["'waste electronics' (kilogram, GLO, None)", -0.00013494676510940288], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 1.1540523311841195e-05]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 4.9787386780698895e-14], ["'Steel cylinder prod.' (unit, GLO, None)", 8.07738375395045e-11], ["'Hydrastic testing 50L' (unit, GLO, None)", 2.8608892926650756e-13], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 9.422194951755147e-14], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 3.0862553071068154e-15], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 1.1984668665162627e-09]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 2.2330865767980447e-11], ["'nitrous oxide production' (kilogram, RER, None)", 1.382679590315926e-10], ["'Cylinder maintenance 50L' (unit, GLO, None)", 4.1366477173536556e-12], ["'Hydrastic testing 50L' (unit, GLO, None)", 2.5748003655596317e-12], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -9.859102191396957e-15], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 5.935472907226001e-11], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 1.9441738208707002e-12], ["'Compresser opration 50L' (unit, GLO, None)", 1.682813673716159e-11]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 3.764871061322028e-11], ["'injection moulding' (kilogram, RER, None)", 2.982129793064838e-14], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 2.56789149717345e-12], ["'market for sodium silicate, solid' (kilogram, RER, None)", 1.1360840966376511e-13], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 9.039094642644986e-12], ["'polypropylene production, granulate' (kilogram, RER, None)", 3.7975284730864555e-14], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 2.1463539482016016e-10], ["'Coating' (kilogram, GLO, None)", 5.90482667800189e-11]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 3.112433080587344e-10], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 3.1124331543316614e-10]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -3.665829878120013e-12], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 2.0729582720289755e-14], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -4.098810725540774e-14], ["'waste electronics' (kilogram, GLO, None)", -4.938960800382458e-12], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", -1.0264979671493479e-13], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 1.0197760284124113e-12]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 8.010363960059452e-11], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 5.434106063788822e-13], ["'injection moulding' (kilogram, RER, None)", 9.088395559550846e-14], ["'market for acetaldehyde' (kilogram, GLO, None)", 1.1027302550449013e-14], ["'market for nylon 6' (kilogram, RER, None)", 2.276941081493087e-14], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 5.135782994220721e-11], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 6.580449061238001e-13], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 3.312828186658051e-11], ["'polypropylene production, granulate' (kilogram, RER, None)", 9.403065317417547e-14], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 7.866387220136538e-10], ["'synthetic rubber production' (kilogram, RER, None)", 9.39722544603925e-13], ["'Coating' (kilogram, GLO, None)", 1.1809653356768508e-10]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 1.1726809313497473e-10], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 1.1726809313784415e-10]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -7.331659756214063e-11], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 6.317587114854775e-14], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -1.5022141309320444e-13], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 2.1536175659711484e-13], ["'waste electronics' (kilogram, GLO, None)", -1.0508427234846831e-11], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 2.039552056846565e-12]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 9.23000990122216e-13], ["'Steel cylinder prod.' (unit, GLO, None)", 5.5583423200027286e-11], ["'Hydrastic testing 50L' (unit, GLO, None)", 8.943190310222103e-12], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 1.7847111486195982e-12], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 1.5679417616712902e-14], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 2.3603623262355048e-08]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase basecase' (unit, GLO, None)", 1.3361670158765134e-08]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 6.063783741777246e-10], ["'nitrous oxide production' (kilogram, RER, None)", 2.7231664930096004e-09], ["'Cylinder maintenance 50L' (unit, GLO, None)", 1.4340113929328455e-10], ["'Hydrastic testing 50L' (unit, GLO, None)", 8.048871302392355e-11], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -4.852931691332586e-14], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 1.1242714381924028e-09], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 9.877184557792858e-12], ["'Compresser opration 50L' (unit, GLO, None)", 3.119743346752718e-10]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 2.2102180258747783e-09], ["'injection moulding' (kilogram, RER, None)", 2.562626756883723e-13], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 1.262675875481751e-10], ["'market for sodium silicate, solid' (kilogram, RER, None)", 3.521336930161632e-12], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 3.045725078428842e-11], ["'polypropylene production, granulate' (kilogram, RER, None)", 8.226152182589259e-13], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 1.6036333357844338e-10], ["'Coating' (kilogram, GLO, None)", 1.996029850253448e-09]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 1.1108940558000346e-08], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 8.559400420214495e-09]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -2.0602743868664676e-10], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 1.1633888888339864e-12], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -2.0175517100923233e-13], ["'waste electronics' (kilogram, GLO, None)", -9.504956408042398e-11], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", 7.834247875926477e-13], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 7.851819466683683e-12]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 4.702591544163575e-09], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 2.5736744730898687e-11], ["'injection moulding' (kilogram, RER, None)", 7.809910113605249e-13], ["'market for acetaldehyde' (kilogram, GLO, None)", 2.830869024833197e-13], ["'market for nylon 6' (kilogram, RER, None)", 2.045325121696746e-13], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 2.5253517510410183e-09], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 1.7537363698696032e-11], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 1.1162582418027227e-10], ["'polypropylene production, granulate' (kilogram, RER, None)", 2.03687863903799e-12], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 5.877316173946279e-10], ["'synthetic rubber production' (kilogram, RER, None)", 1.819106515258094e-11], ["'Coating' (kilogram, GLO, None)", 3.992059701550503e-09]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 5.7744917398854014e-09], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 3.2249513995028613e-09]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -4.120548773785221e-09], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 3.5455661375173752e-12], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -7.39432701804302e-13], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 1.1017254260623163e-11], ["'waste electronics' (kilogram, GLO, None)", -2.0223311506361686e-10], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 1.5703638936115418e-11]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 4.9748432120241335e-06], ["'Steel cylinder prod.' (unit, GLO, None)", -7.122968863629567e-05], ["'Hydrastic testing 50L' (unit, GLO, None)", 9.984953097054036e-05], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 8.851887766613423e-07], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 3.414766387261568e-08], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 0.36859257084241986]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 0.0065511156330904955], ["'nitrous oxide production' (kilogram, RER, None)", 0.04252478220335179], ["'Cylinder maintenance 50L' (unit, GLO, None)", -1.6954339060072137e-05], ["'Hydrastic testing 50L' (unit, GLO, None)", 0.0008986457788096962], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -2.3945055594087172e-08], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.0005576210244715975], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 2.1511180229247912e-05], ["'Compresser opration 50L' (unit, GLO, None)", 0.0016814970056216606]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.0031690392104530164], ["'injection moulding' (kilogram, RER, None)", 5.203950693096914e-06], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.00033008017268783583], ["'market for sodium silicate, solid' (kilogram, RER, None)", -1.122635412057962e-05], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.0001362665733797331], ["'polypropylene production, granulate' (kilogram, RER, None)", 2.633843639547243e-06], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", -0.00037479559560256134], ["'Coating' (kilogram, GLO, None)", 0.01969643205028478]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 0.00034780368107774893], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.0003478036893232272]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 1.4146034376022545e-05], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 4.837811316788339e-06], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -9.954887247426905e-08], ["'waste electronics' (kilogram, GLO, None)", 8.643488712410244e-05], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", 1.5284126258662182e-06], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 4.231149122808276e-06]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.006742636617970905], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 1.6149217476118665e-06], ["'injection moulding' (kilogram, RER, None)", 1.5859659255167497e-05], ["'market for acetaldehyde' (kilogram, GLO, None)", 7.715345946734232e-07], ["'market for nylon 6' (kilogram, RER, None)", 8.16868929853253e-09], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.006601603453788899], ["'market for sodium silicate, solid' (kilogram, RoW, None)", -8.862520601462733e-05], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.0004994169914241051], ["'polypropylene production, granulate' (kilogram, RER, None)", 6.521663748700984e-06], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", -0.0013736258578935325], ["'synthetic rubber production' (kilogram, RER, None)", 6.861108366864148e-05], ["'Coating' (kilogram, GLO, None)", 0.039392864100563835]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 0.00013104305669854347], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.00013104305670393648]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 0.00028292068752524304], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 1.4743805917831063e-05], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -3.648466176338076e-07], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 3.132092631634113e-05], ["'waste electronics' (kilogram, GLO, None)", 0.00018390401515833315], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 8.462298245613712e-06]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 0.00035345078353973646], ["'Steel cylinder prod.' (unit, GLO, None)", 0.04494169943077192], ["'Hydrastic testing 50L' (unit, GLO, None)", 0.006551456902773902], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.001523022869315982], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 4.095196497538135e-05], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 24.97652679032572]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 0.4925080636167122], ["'nitrous oxide production' (kilogram, RER, None)", 2.8815593295700435], ["'Cylinder maintenance 50L' (unit, GLO, None)", 0.01570278749644992], ["'Hydrastic testing 50L' (unit, GLO, None)", 0.05896311203876186], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -1.3981777829394786e-05], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.9594219844056571], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 0.025797521688597138], ["'Compresser opration 50L' (unit, GLO, None)", 0.11946636493364346]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.3129543732766188], ["'injection moulding' (kilogram, RER, None)", -0.00019978258866021033], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.025671851494819202], ["'market for sodium silicate, solid' (kilogram, RER, None)", 0.0033571907315621758], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.01999905702319062], ["'polypropylene production, granulate' (kilogram, RER, None)", 0.00026573726284582306], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.1481970574621222], ["'Coating' (kilogram, GLO, None)", 0.935113903561229]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 30.062931903317136], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 30.06293261441621]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -0.014964564895088378], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 0.003671331284741333], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -5.812766701665658e-05], ["'waste electronics' (kilogram, GLO, None)", -0.016854079220950467], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", -0.0007395422745039993], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.0006203265676319966]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.6658603699920232], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", -0.009462532141128974], ["'injection moulding' (kilogram, RER, None)", -0.0006088612225432471], ["'market for acetaldehyde' (kilogram, GLO, None)", 0.00019882091526749588], ["'market for nylon 6' (kilogram, RER, None)", -1.7267134839775114e-05], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.5134370298941939], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 0.02331116045304413], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.07329654411420672], ["'polypropylene production, granulate' (kilogram, RER, None)", 0.0006579923908499737], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.543142215560722], ["'synthetic rubber production' (kilogram, RER, None)", 0.010052683430200021], ["'Coating' (kilogram, GLO, None)", 1.8702278080765016]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 11.326902802631512], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 11.326902802428581]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -0.2992912979088652], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 0.011188819153602972], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -0.00021303789959449586], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.02468743834151873], ["'waste electronics' (kilogram, GLO, None)", -0.03585974309532576], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.0012406531360487018]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 1.4770963355147075e-09], ["'Steel cylinder prod.' (unit, GLO, None)", -7.476008903801536e-08], ["'Hydrastic testing 50L' (unit, GLO, None)", 1.0334066734325901e-08], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 3.4417450302031337e-10], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", -3.230975077255589e-12], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 3.060770115022358e-05]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 7.511332906692129e-07], ["'nitrous oxide production' (kilogram, RER, None)", 3.5312318481114463e-06], ["'Cylinder maintenance 50L' (unit, GLO, None)", 3.533949686944155e-08], ["'Hydrastic testing 50L' (unit, GLO, None)", 9.300660063252953e-08], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", 4.978452590961879e-11], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 2.168113107877337e-07], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", -2.035339443901625e-09], ["'Compresser opration 50L' (unit, GLO, None)", 4.992585612621846e-07]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 1.4462347185828065e-05], ["'injection moulding' (kilogram, RER, None)", -8.198311069246805e-12], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 1.6311398279135516e-06], ["'market for sodium silicate, solid' (kilogram, RER, None)", 4.2157297272018545e-09], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", -6.163301770416577e-08], ["'polypropylene production, granulate' (kilogram, RER, None)", 1.3411662583252743e-09], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 3.706229506327243e-08], ["'Coating' (kilogram, GLO, None)", 7.130292587666517e-06]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 9.73441196893503e-06], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 9.734412199711486e-06]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -1.3450730237410633e-07], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 1.3548324618470628e-11], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", 2.0697356087496828e-10], ["'waste electronics' (kilogram, GLO, None)", 8.879458202554093e-07], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", -8.99139681593359e-09], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", -3.8670289502216895e-09]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 3.0770951459210686e-05], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", -3.428967624699589e-09], ["'injection moulding' (kilogram, RER, None)", -2.498532898419031e-11], ["'market for acetaldehyde' (kilogram, GLO, None)", 2.581070275156109e-10], ["'market for nylon 6' (kilogram, RER, None)", 1.837779987399219e-09], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 3.2622796558278885e-05], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 2.4401194188988863e-08], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", -2.25885009896268e-07], ["'polypropylene production, granulate' (kilogram, RER, None)", 3.3208635609584262e-09], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 1.3583331142843333e-07], ["'synthetic rubber production' (kilogram, RER, None)", 3.076772824665024e-08], ["'Coating' (kilogram, GLO, None)", 1.4260585175207938e-05]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 3.6676641708639582e-06], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 3.6676641709913554e-06]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", -2.69014604749345e-06], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 4.129013216967817e-11], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", 7.585581005536807e-10], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 6.456437731471709e-11], ["'waste electronics' (kilogram, GLO, None)", 1.889246426075327e-06], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", -7.734057900462786e-09]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 5.46795457621353e-13], ["'Steel cylinder prod.' (unit, GLO, None)", 1.0455303815707074e-10], ["'Hydrastic testing 50L' (unit, GLO, None)", 1.4162901197208436e-11], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 3.918373210477902e-12], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 8.657384061920889e-14], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 7.399666015179285e-08]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 1.047100938094354e-09], ["'nitrous oxide production' (kilogram, RER, None)", 8.53704633722511e-09], ["'Cylinder maintenance 50L' (unit, GLO, None)", 9.190957331363661e-08], ["'Hydrastic testing 50L' (unit, GLO, None)", 1.274661107693019e-10], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -4.894332461938955e-13], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 2.4683630672880778e-09], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 5.453683436856975e-11], ["'Compresser opration 50L' (unit, GLO, None)", 1.8481686467403636e-10]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 3.10958022670216e-09], ["'injection moulding' (kilogram, RER, None)", 3.7436449497269617e-11], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 2.770138718782797e-10], ["'market for sodium silicate, solid' (kilogram, RER, None)", 1.9904368631179006e-12], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 1.2528918864867743e-10], ["'polypropylene production, granulate' (kilogram, RER, None)", 1.2588253851343943e-12], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 2.45452805439037e-10], ["'Coating' (kilogram, GLO, None)", 2.6141665308790514e-09]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 1.9450074604811147e-09], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 1.9450075064659068e-09]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 4.2594749861336265e-13], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", -3.787390348810768e-13], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -2.034763613067223e-12], ["'waste electronics' (kilogram, GLO, None)", 1.12696348819e-11], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", 1.0922054233770265e-13], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 3.717467338180751e-12]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 6.6161281419695575e-09], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 4.318811743424509e-11], ["'injection moulding' (kilogram, RER, None)", 1.1409203656280585e-10], ["'market for acetaldehyde' (kilogram, GLO, None)", 2.055323735271043e-13], ["'market for nylon 6' (kilogram, RER, None)", 4.432438863312134e-14], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 5.540277437336517e-09], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 5.329331413581773e-12], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 4.591848764271115e-10], ["'polypropylene production, granulate' (kilogram, RER, None)", 3.1169792151620525e-12], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 8.995845319172511e-10], ["'synthetic rubber production' (kilogram, RER, None)", 5.327583237248117e-11], ["'Coating' (kilogram, GLO, None)", 5.228333061776189e-09]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 7.328264098056545e-10], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 7.328264098097583e-10]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 8.518950142536406e-12], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", -1.154252296527102e-12], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -7.45740864070404e-12], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", -4.64822063429864e-12], ["'waste electronics' (kilogram, GLO, None)", 2.3977946552986694e-11], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 7.434934677086305e-12]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 6.219819895879126e-13], ["'Steel cylinder prod.' (unit, GLO, None)", 5.251274388894696e-10], ["'Hydrastic testing 50L' (unit, GLO, None)", 9.537640509260688e-12], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 1.229225909281124e-11], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 9.522275491675729e-14], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 5.122923506338801e-08]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 9.106749191072184e-10], ["'nitrous oxide production' (kilogram, RER, None)", 5.910352611610113e-09], ["'Cylinder maintenance 50L' (unit, GLO, None)", 1.1350495269355735e-09], ["'Hydrastic testing 50L' (unit, GLO, None)", 8.583876459395599e-11], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -7.393946755952687e-12], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 7.74345799342058e-09], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 5.998518231262449e-11], ["'Compresser opration 50L' (unit, GLO, None)", 2.1022991242518374e-10]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 1.5252161448878907e-09], ["'injection moulding' (kilogram, RER, None)", 8.539214850326713e-13], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 1.887556151112882e-10], ["'market for sodium silicate, solid' (kilogram, RER, None)", 4.554212662764161e-12], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 1.437020422393877e-10], ["'polypropylene production, granulate' (kilogram, RER, None)", 5.109361027561149e-12], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 5.264876269729494e-10], ["'Coating' (kilogram, GLO, None)", 2.679629713734777e-08]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 1.3992546508923827e-08], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 1.3992546840482602e-08]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 1.3902273685457593e-10], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 2.219629332485331e-12], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -3.073950109966252e-11], ["'waste electronics' (kilogram, GLO, None)", 5.994688597951452e-10], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", 1.1444955092336274e-11], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 4.306994856184459e-11]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 3.245140733808002e-09], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 2.0689613006568184e-10], ["'injection moulding' (kilogram, RER, None)", 2.6024273829534647e-12], ["'market for acetaldehyde' (kilogram, GLO, None)", 1.1482011932869868e-12], ["'market for nylon 6' (kilogram, RER, None)", 1.1301029977656342e-11], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 3.7751123022027275e-09], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 2.7388875761821727e-11], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 5.266679848175202e-10], ["'polypropylene production, granulate' (kilogram, RER, None)", 1.265129565492596e-11], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 1.9295771528619285e-09], ["'synthetic rubber production' (kilogram, RER, None)", 9.061419767149456e-11], ["'Coating' (kilogram, GLO, None)", 5.359259427464247e-08]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 5.272014545275251e-09], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 5.272014545394584e-09]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 2.780454737100439e-09], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 6.764584632336048e-12], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -1.1266027153029697e-10], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 1.3070299709142706e-11], ["'waste electronics' (kilogram, GLO, None)", 1.27546565913862e-09], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 8.613989712367268e-11]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 6.410978177017208e-08], ["'Steel cylinder prod.' (unit, GLO, None)", 2.1650696275927872e-05], ["'Hydrastic testing 50L' (unit, GLO, None)", 9.855466271346733e-07], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 5.87844785011443e-07], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 5.31448477191255e-08], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 0.006123632180781964]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 8.847286934611855e-05], ["'nitrous oxide production' (kilogram, RER, None)", 0.0007064877194818821], ["'Cylinder maintenance 50L' (unit, GLO, None)", 3.850296735636573e-05], ["'Hydrastic testing 50L' (unit, GLO, None)", 8.869919644739004e-06], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -3.9828812604595554e-07], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.0003703104014499124], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 3.3478377959048045e-05], ["'Compresser opration 50L' (unit, GLO, None)", 2.16691062367689e-05]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.00014758440666929443], ["'injection moulding' (kilogram, RER, None)", 2.26592733479606e-07], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 1.6985305443423847e-05], ["'market for sodium silicate, solid' (kilogram, RER, None)", 4.425330357788671e-07], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 1.2692902073607448e-05], ["'polypropylene production, granulate' (kilogram, RER, None)", 4.4232247469428165e-07], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 5.321277833276502e-05], ["'Coating' (kilogram, GLO, None)", 0.002446814008015474]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 0.0008604984653242085], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.0008604984857116755]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 9.233578875873739e-06], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 2.4875742545946803e-07], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -1.6558380378813868e-06], ["'waste electronics' (kilogram, GLO, None)", 4.419094480096524e-05], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", 7.41212024600797e-07], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 1.8773728433315984e-06]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.0003140093758922613], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 9.065147547057334e-06], ["'injection moulding' (kilogram, RER, None)", 6.905683306040559e-07], ["'market for acetaldehyde' (kilogram, GLO, None)", 1.049154914409454e-07], ["'market for nylon 6' (kilogram, RER, None)", 7.804538237294221e-07], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.000339706108865833], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 2.478087926770315e-06], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 4.6519486100823134e-05], ["'polypropylene production, granulate' (kilogram, RER, None)", 1.0952352695339758e-06], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.0001950248325899108], ["'synthetic rubber production' (kilogram, RER, None)", 7.851567027533186e-06], ["'Coating' (kilogram, GLO, None)", 0.004893628016027952]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 0.000324212638670387], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.00032421263867682805]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 0.00018467157751811647], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 7.581178680669171e-07], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -6.06864640883731e-06], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 1.5858343796344777e-06], ["'waste electronics' (kilogram, GLO, None)", 9.402328681056596e-05], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 3.754745686660822e-06]]</t>
+  </si>
+  <si>
+    <t>[["'Compresser opration 50L' (unit, GLO, None)", 5.304401344811386e-06], ["'Steel cylinder prod.' (unit, GLO, None)", 0.0013982425312678971], ["'Hydrastic testing 50L' (unit, GLO, None)", 0.00010074041304536374], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 1.1125396265905287e-05], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 3.0469015546991656e-07], ["'nitrous oxide production' (kilogram, RER, None)", 0.0]]</t>
+  </si>
+  <si>
+    <t>[["'nitrous oxide production' (kilogram, RER, None)", 3.8432817789367]]</t>
+  </si>
+  <si>
+    <t>[["'Cylinder cleaning 50L' (unit, GLO, None)", 0.01448393596929188], ["'nitrous oxide production' (kilogram, RER, None)", 0.44340210173684325], ["'Cylinder maintenance 50L' (unit, GLO, None)", 0.0021593015629354038], ["'Hydrastic testing 50L' (unit, GLO, None)", 0.0009066637174049738], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -7.634788455592453e-07], ["'transport, freight, lorry 16-32 metric ton, EURO6' (ton kilometer, RER, None)", 0.00700839756098478], ["'transport, freight, inland waterways, barge tanker' (ton kilometer, RER, None)", 0.00019193830866054903], ["'Compresser opration 50L' (unit, GLO, None)", 0.0017928876545482168]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.011234107352487532], ["'injection moulding' (kilogram, RER, None)", 2.7960201290127477e-05], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.0011855045386309408], ["'market for sodium silicate, solid' (kilogram, RER, None)", 0.00013952613085102148], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.0009977849386785698], ["'polypropylene production, granulate' (kilogram, RER, None)", 4.7452982786098155e-05], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.003230971428962673], ["'Coating' (kilogram, GLO, None)", 0.029238904020596285]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase CDU' (unit, GLO, None)", 0.026577952306826722], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.026577952936570594]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 0.000139380474162897], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 3.326127925921901e-05], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -3.1740773348402537e-06], ["'waste electronics' (kilogram, GLO, None)", 0.0005824459279498765], ["'treatment of used liquid crystal display, mechanical treatment' (kilogram, GLO, None)", 1.6513453462663282e-05], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.00012918336066532695]]</t>
+  </si>
+  <si>
+    <t>[["'Electronics' (kilogram, GLO, None)", 0.023902356069129896], ["'activated carbon production, granular from hard coal' (kilogram, RER, None)", 9.33673915764238e-05], ["'injection moulding' (kilogram, RER, None)", 8.521204202701847e-05], ["'market for acetaldehyde' (kilogram, GLO, None)", 2.0521046126214145e-05], ["'market for nylon 6' (kilogram, RER, None)", 8.20330292729018e-05], ["'market for printed wiring board, surface mounted, unspecified, Pb free' (kilogram, GLO, None)", 0.023710090772472145], ["'market for sodium silicate, solid' (kilogram, RoW, None)", 0.0007672676837867333], ["'metal working, average for steel product manufacturing' (kilogram, RER, None)", 0.0036568818003163686], ["'polypropylene production, granulate' (kilogram, RER, None)", 0.00011749839396635427], ["'steel production, chromium steel 18/8, hot rolled' (kilogram, RER, None)", 0.011841510287167116], ["'synthetic rubber production' (kilogram, RER, None)", 0.0009378584068275059], ["'Coating' (kilogram, GLO, None)", 0.05847780804109285]]</t>
+  </si>
+  <si>
+    <t>[["'Use phase MDU' (unit, GLO, None)", 0.01001385638102837], ["'market for electricity, low voltage' (kilowatt hour, DK, None)", 0.010013856381243535]]</t>
+  </si>
+  <si>
+    <t>[["'treatment of scrap printed wiring boards, shredding and separation' (kilogram, RoW, None)", 0.002787609483278382], ["'treatment of waste plastic, mixture, municipal incineration' (kilogram, RoW, None)", 0.00010136770821857213], ["'treatment of waste reinforcement steel, recycling' (kilogram, RoW, None)", -1.1632993432276693e-05], ["'treatment of waste rubber, unspecified, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.0001890127801177668], ["'waste electronics' (kilogram, GLO, None)", 0.0012392466552126743], ["'treatment of scrap aluminium, municipal incineration' (kilogram, Europe without Switzerland, None)", 0.0002583667213305514]]</t>
   </si>
 </sst>
 </file>
@@ -563,7 +860,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -624,49 +921,49 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="J2" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>109</v>
       </c>
       <c r="L2" t="s">
-        <v>49</v>
+        <v>118</v>
       </c>
       <c r="M2" t="s">
-        <v>52</v>
+        <v>127</v>
       </c>
       <c r="N2" t="s">
-        <v>55</v>
+        <v>136</v>
       </c>
       <c r="O2" t="s">
-        <v>58</v>
+        <v>145</v>
       </c>
       <c r="P2" t="s">
-        <v>61</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -674,49 +971,49 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>101</v>
       </c>
       <c r="K3" t="s">
-        <v>47</v>
+        <v>110</v>
       </c>
       <c r="L3" t="s">
-        <v>50</v>
+        <v>119</v>
       </c>
       <c r="M3" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="N3" t="s">
-        <v>56</v>
+        <v>137</v>
       </c>
       <c r="O3" t="s">
-        <v>59</v>
+        <v>146</v>
       </c>
       <c r="P3" t="s">
-        <v>62</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -724,49 +1021,699 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" t="s">
+        <v>93</v>
+      </c>
+      <c r="J5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K5" t="s">
+        <v>111</v>
+      </c>
+      <c r="L5" t="s">
+        <v>120</v>
+      </c>
+      <c r="M5" t="s">
+        <v>129</v>
+      </c>
+      <c r="N5" t="s">
+        <v>138</v>
+      </c>
+      <c r="O5" t="s">
+        <v>147</v>
+      </c>
+      <c r="P5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K6" t="s">
+        <v>112</v>
+      </c>
+      <c r="L6" t="s">
+        <v>121</v>
+      </c>
+      <c r="M6" t="s">
+        <v>130</v>
+      </c>
+      <c r="N6" t="s">
+        <v>139</v>
+      </c>
+      <c r="O6" t="s">
+        <v>148</v>
+      </c>
+      <c r="P6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" t="s">
+        <v>100</v>
+      </c>
+      <c r="K7" t="s">
+        <v>109</v>
+      </c>
+      <c r="L7" t="s">
+        <v>118</v>
+      </c>
+      <c r="M7" t="s">
+        <v>127</v>
+      </c>
+      <c r="N7" t="s">
+        <v>136</v>
+      </c>
+      <c r="O7" t="s">
+        <v>145</v>
+      </c>
+      <c r="P7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" t="s">
+        <v>55</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8" t="s">
+        <v>110</v>
+      </c>
+      <c r="L8" t="s">
+        <v>119</v>
+      </c>
+      <c r="M8" t="s">
+        <v>128</v>
+      </c>
+      <c r="N8" t="s">
+        <v>137</v>
+      </c>
+      <c r="O8" t="s">
+        <v>146</v>
+      </c>
+      <c r="P8" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" t="s">
+        <v>113</v>
+      </c>
+      <c r="L9" t="s">
+        <v>122</v>
+      </c>
+      <c r="M9" t="s">
+        <v>131</v>
+      </c>
+      <c r="N9" t="s">
+        <v>140</v>
+      </c>
+      <c r="O9" t="s">
+        <v>149</v>
+      </c>
+      <c r="P9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" t="s">
+        <v>105</v>
+      </c>
+      <c r="K10" t="s">
+        <v>114</v>
+      </c>
+      <c r="L10" t="s">
+        <v>123</v>
+      </c>
+      <c r="M10" t="s">
+        <v>132</v>
+      </c>
+      <c r="N10" t="s">
+        <v>141</v>
+      </c>
+      <c r="O10" t="s">
+        <v>150</v>
+      </c>
+      <c r="P10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
+        <v>83</v>
+      </c>
+      <c r="I11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" t="s">
+        <v>111</v>
+      </c>
+      <c r="L11" t="s">
+        <v>120</v>
+      </c>
+      <c r="M11" t="s">
+        <v>129</v>
+      </c>
+      <c r="N11" t="s">
+        <v>138</v>
+      </c>
+      <c r="O11" t="s">
+        <v>147</v>
+      </c>
+      <c r="P11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" t="s">
+        <v>87</v>
+      </c>
+      <c r="I12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J12" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" t="s">
+        <v>115</v>
+      </c>
+      <c r="L12" t="s">
+        <v>124</v>
+      </c>
+      <c r="M12" t="s">
+        <v>133</v>
+      </c>
+      <c r="N12" t="s">
+        <v>142</v>
+      </c>
+      <c r="O12" t="s">
+        <v>151</v>
+      </c>
+      <c r="P12" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" t="s">
+        <v>100</v>
+      </c>
+      <c r="K13" t="s">
+        <v>109</v>
+      </c>
+      <c r="L13" t="s">
+        <v>118</v>
+      </c>
+      <c r="M13" t="s">
+        <v>127</v>
+      </c>
+      <c r="N13" t="s">
+        <v>136</v>
+      </c>
+      <c r="O13" t="s">
+        <v>145</v>
+      </c>
+      <c r="P13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" t="s">
+        <v>82</v>
+      </c>
+      <c r="I14" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" t="s">
+        <v>101</v>
+      </c>
+      <c r="K14" t="s">
+        <v>110</v>
+      </c>
+      <c r="L14" t="s">
+        <v>119</v>
+      </c>
+      <c r="M14" t="s">
+        <v>128</v>
+      </c>
+      <c r="N14" t="s">
+        <v>137</v>
+      </c>
+      <c r="O14" t="s">
+        <v>146</v>
+      </c>
+      <c r="P14" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" t="s">
-        <v>45</v>
-      </c>
-      <c r="K4" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" t="s">
-        <v>51</v>
-      </c>
-      <c r="M4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N4" t="s">
-        <v>57</v>
-      </c>
-      <c r="O4" t="s">
-        <v>60</v>
-      </c>
-      <c r="P4" t="s">
-        <v>63</v>
+      <c r="B15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" t="s">
+        <v>98</v>
+      </c>
+      <c r="J15" t="s">
+        <v>107</v>
+      </c>
+      <c r="K15" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" t="s">
+        <v>125</v>
+      </c>
+      <c r="M15" t="s">
+        <v>134</v>
+      </c>
+      <c r="N15" t="s">
+        <v>143</v>
+      </c>
+      <c r="O15" t="s">
+        <v>152</v>
+      </c>
+      <c r="P15" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J16" t="s">
+        <v>108</v>
+      </c>
+      <c r="K16" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" t="s">
+        <v>126</v>
+      </c>
+      <c r="M16" t="s">
+        <v>135</v>
+      </c>
+      <c r="N16" t="s">
+        <v>144</v>
+      </c>
+      <c r="O16" t="s">
+        <v>153</v>
+      </c>
+      <c r="P16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" t="s">
+        <v>83</v>
+      </c>
+      <c r="I17" t="s">
+        <v>93</v>
+      </c>
+      <c r="J17" t="s">
+        <v>102</v>
+      </c>
+      <c r="K17" t="s">
+        <v>111</v>
+      </c>
+      <c r="L17" t="s">
+        <v>120</v>
+      </c>
+      <c r="M17" t="s">
+        <v>129</v>
+      </c>
+      <c r="N17" t="s">
+        <v>138</v>
+      </c>
+      <c r="O17" t="s">
+        <v>147</v>
+      </c>
+      <c r="P17" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>